<commit_message>
Improved JSON Utility and minor changes in external/results API caller
</commit_message>
<xml_diff>
--- a/public/files/storage/Storage_Bulk_Upload_Excel_Format.xlsx
+++ b/public/files/storage/Storage_Bulk_Upload_Excel_Format.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="7">
   <si>
     <t>Sample Code</t>
   </si>
@@ -36,117 +36,6 @@
   </si>
   <si>
     <t>Volume (ml)</t>
-  </si>
-  <si>
-    <t>VL07248801</t>
-  </si>
-  <si>
-    <t>NW/39/01/19/0001</t>
-  </si>
-  <si>
-    <t>VL08248803</t>
-  </si>
-  <si>
-    <t>VL08248804</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>VL08248805</t>
-  </si>
-  <si>
-    <t>Domla</t>
-  </si>
-  <si>
-    <t>VL08248806</t>
-  </si>
-  <si>
-    <t>SDSDSD</t>
-  </si>
-  <si>
-    <t>VL08248807</t>
-  </si>
-  <si>
-    <t>S3rdfr</t>
-  </si>
-  <si>
-    <t>VL08248808</t>
-  </si>
-  <si>
-    <t>sewrewrer</t>
-  </si>
-  <si>
-    <t>VL08248809</t>
-  </si>
-  <si>
-    <t>errererer</t>
-  </si>
-  <si>
-    <t>VL08248810</t>
-  </si>
-  <si>
-    <t>er3erer</t>
-  </si>
-  <si>
-    <t>VL08248811</t>
-  </si>
-  <si>
-    <t>Chsudhj</t>
-  </si>
-  <si>
-    <t>VL08248812</t>
-  </si>
-  <si>
-    <t>SCdf</t>
-  </si>
-  <si>
-    <t>VL08248813</t>
-  </si>
-  <si>
-    <t>SX</t>
-  </si>
-  <si>
-    <t>VL08248814</t>
-  </si>
-  <si>
-    <t>SDSDSDSDDDSD</t>
-  </si>
-  <si>
-    <t>VL08248824</t>
-  </si>
-  <si>
-    <t>VL08248825</t>
-  </si>
-  <si>
-    <t>VL08248826</t>
-  </si>
-  <si>
-    <t>VL08248827</t>
-  </si>
-  <si>
-    <t>VL08248833</t>
-  </si>
-  <si>
-    <t>G8h</t>
-  </si>
-  <si>
-    <t>VL08248834</t>
-  </si>
-  <si>
-    <t>X898</t>
-  </si>
-  <si>
-    <t>VL08248835</t>
-  </si>
-  <si>
-    <t>TOMO2</t>
-  </si>
-  <si>
-    <t>VL08248836</t>
-  </si>
-  <si>
-    <t>SW/07/12/20/001</t>
   </si>
 </sst>
 </file>
@@ -541,7 +430,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:AMJ22"/>
+  <dimension ref="A1:AMJ1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1" topLeftCell="A1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1603,162 +1492,6 @@
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
     </row>
-    <row r="2" spans="1:1024">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1024">
-      <c r="A3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3333333</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1024">
-      <c r="A4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1024">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1024">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1024">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1024">
-      <c r="A8" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1024">
-      <c r="A9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1024">
-      <c r="A10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1024">
-      <c r="A11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1024">
-      <c r="A12" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1024">
-      <c r="A13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1024">
-      <c r="A14" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1024">
-      <c r="A15" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1024">
-      <c r="A16" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1024">
-      <c r="A17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1024">
-      <c r="A18" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1024">
-      <c r="A19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1024">
-      <c r="A20" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1024">
-      <c r="A21" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1024">
-      <c r="A22" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>43</v>
-      </c>
-    </row>
   </sheetData>
   <printOptions gridLines="false" gridLinesSet="true"/>
   <pageMargins left="0.7875" right="0.7875" top="1.0527777777778" bottom="1.0527777777778" header="0.7875" footer="0.7875"/>

</xml_diff>